<commit_message>
added note to descriptions end date field
</commit_message>
<xml_diff>
--- a/18th_cent_descriptions_fields.xlsx
+++ b/18th_cent_descriptions_fields.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Commissaire-Pr.</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>YYYY MM DD or "and following days"…</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -572,7 +575,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
+        <f t="shared" ref="C2:C21" si="0">SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
         <v>auction_house</v>
       </c>
     </row>
@@ -584,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B3)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>auctioneer_copy</v>
       </c>
     </row>
@@ -596,7 +599,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B4)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>authority_city</v>
       </c>
     </row>
@@ -608,7 +611,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B5)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>catalog_location</v>
       </c>
     </row>
@@ -620,7 +623,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B6)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>catalogue_number</v>
       </c>
     </row>
@@ -632,7 +635,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B7)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>commissaire_priseur</v>
       </c>
       <c r="D7" t="s">
@@ -647,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B8)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>country</v>
       </c>
       <c r="D8" t="s">
@@ -662,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B9)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>expert</v>
       </c>
     </row>
@@ -674,7 +677,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B10)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>lugt_number</v>
       </c>
     </row>
@@ -686,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B11)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>notes</v>
       </c>
     </row>
@@ -698,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="C12" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B12)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>number_of_lots</v>
       </c>
       <c r="F12" t="s">
@@ -713,7 +716,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B13)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>other_sellers</v>
       </c>
       <c r="D13" t="s">
@@ -728,7 +731,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B14)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>photocopies</v>
       </c>
     </row>
@@ -740,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B15)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>sale_begin_date</v>
       </c>
       <c r="F15" t="s">
@@ -758,14 +761,14 @@
         <v>11</v>
       </c>
       <c r="C16" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B16)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>sale_end_date</v>
       </c>
       <c r="F16" t="s">
         <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -776,7 +779,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B17)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>sale_location</v>
       </c>
     </row>
@@ -788,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B18)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>seller_authority</v>
       </c>
       <c r="D18" t="s">
@@ -803,7 +806,7 @@
         <v>29</v>
       </c>
       <c r="C19" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B19)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>specific_location</v>
       </c>
     </row>
@@ -815,7 +818,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>title_page</v>
       </c>
     </row>
@@ -827,7 +830,7 @@
         <v>27</v>
       </c>
       <c r="C21" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B21)," ","_"),"-","_")</f>
+        <f t="shared" si="0"/>
         <v>verbatim_auction_house</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mods to sales description parsing and MongoDB scripts
</commit_message>
<xml_diff>
--- a/18th_cent_descriptions_fields.xlsx
+++ b/18th_cent_descriptions_fields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Commissaire-Pr.</t>
   </si>
@@ -130,6 +130,42 @@
   </si>
   <si>
     <t>YYYY MM DD or "and following days"…</t>
+  </si>
+  <si>
+    <t>Verbatim Expert</t>
+  </si>
+  <si>
+    <t>Expert Authority</t>
+  </si>
+  <si>
+    <t>Verb.Comm.-Pris.</t>
+  </si>
+  <si>
+    <t>Comm.-Pris.Auth.</t>
+  </si>
+  <si>
+    <t>Verb.Auct. House</t>
+  </si>
+  <si>
+    <t>Auct.House Auth</t>
+  </si>
+  <si>
+    <t>Verbatim Commissaire-Priseur</t>
+  </si>
+  <si>
+    <t>Commissaire-Priseur Authority</t>
+  </si>
+  <si>
+    <t>Auction House Authority</t>
+  </si>
+  <si>
+    <t>expert_info</t>
+  </si>
+  <si>
+    <t>auction_house_info</t>
+  </si>
+  <si>
+    <t>commissaire_priseur_info</t>
   </si>
 </sst>
 </file>
@@ -186,8 +222,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -195,9 +243,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,19 +587,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
   </cols>
@@ -575,149 +635,173 @@
         <v>14</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C21" si="0">SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
+        <f t="shared" ref="C2:C27" si="0">SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
         <v>auction_house</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>auctioneer_copy</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B3)," ","_"),"-","_")</f>
+        <v>verbatim_auction_house</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>authority_city</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B4)," ","_"),"-","_")</f>
+        <v>verbatim_auction_house</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>catalog_location</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B5)," ","_"),"-","_")</f>
+        <v>auction_house_authority</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>catalogue_number</v>
+        <v>auctioneer_copy</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>commissaire_priseur</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
+        <v>authority_city</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>country</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
+        <v>catalog_location</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>expert</v>
+        <v>catalogue_number</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>lugt_number</v>
+        <v>commissaire_priseur</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>notes</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B11)," ","_"),"-","_")</f>
+        <v>verbatim_commissaire_priseur</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>number_of_lots</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B12)," ","_"),"-","_")</f>
+        <v>commissaire_priseur_authority</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>other_sellers</v>
+        <v>country</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -725,113 +809,203 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>photocopies</v>
+        <v>expert</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>sale_begin_date</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>34</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B15)," ","_"),"-","_")</f>
+        <v>verbatim_expert</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B16)," ","_"),"-","_")</f>
+        <v>expert_authority</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>lugt_number</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>number_of_lots</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>other_sellers</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>photocopies</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>sale_begin_date</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>sale_end_date</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F23" t="s">
         <v>33</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>sale_location</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>seller_authority</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>specific_location</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>title_page</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>verbatim_auction_house</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now parsing sales contents, too
</commit_message>
<xml_diff>
--- a/18th_cent_descriptions_fields.xlsx
+++ b/18th_cent_descriptions_fields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18400" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Commissaire-Pr.</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>commissaire_priseur_info</t>
+  </si>
+  <si>
+    <t>Country Auth.</t>
+  </si>
+  <si>
+    <t>Country Authority</t>
+  </si>
+  <si>
+    <t>Edit Status</t>
   </si>
 </sst>
 </file>
@@ -222,8 +231,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -243,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -251,6 +264,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -258,6 +273,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -635,7 +652,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C27" si="0">SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
+        <f t="shared" ref="C2:C29" si="0">SUBSTITUTE(SUBSTITUTE(LOWER(B2)," ","_"),"-","_")</f>
         <v>auction_house</v>
       </c>
     </row>
@@ -800,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C13" si="1">SUBSTITUTE(SUBSTITUTE(LOWER(B13)," ","_"),"-","_")</f>
         <v>country</v>
       </c>
       <c r="D13" t="s">
@@ -809,44 +826,38 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>expert</v>
+        <v>country_authority</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B15)," ","_"),"-","_")</f>
-        <v>verbatim_expert</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>expert</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(B16)," ","_"),"-","_")</f>
-        <v>expert_authority</v>
+        <v>verbatim_expert</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -857,155 +868,185 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>lugt_number</v>
+        <f>SUBSTITUTE(SUBSTITUTE(LOWER(B17)," ","_"),"-","_")</f>
+        <v>expert_authority</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>notes</v>
+        <v>lugt_number</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>number_of_lots</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
+        <v>notes</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>other_sellers</v>
-      </c>
-      <c r="D20" t="s">
-        <v>32</v>
+        <v>number_of_lots</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>photocopies</v>
+        <v>other_sellers</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>sale_begin_date</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" t="s">
-        <v>34</v>
+        <v>photocopies</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>sale_end_date</v>
+        <v>sale_begin_date</v>
       </c>
       <c r="F23" t="s">
         <v>33</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>sale_location</v>
+        <v>sale_end_date</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>seller_authority</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
+        <v>sale_location</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>specific_location</v>
+        <v>seller_authority</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>specific_location</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>16</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>title_page</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_status</v>
       </c>
     </row>
   </sheetData>

</xml_diff>